<commit_message>
Reducción a archivos escenciales
eliminar archivos que no son necesarios para generar las instancias o correr el modelo.
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>FO</t>
   </si>
@@ -43,7 +43,13 @@
     <t>Time</t>
   </si>
   <si>
-    <t>20x4_1</t>
+    <t>10x2_1</t>
+  </si>
+  <si>
+    <t>10x2_2</t>
+  </si>
+  <si>
+    <t>10x2_3</t>
   </si>
 </sst>
 </file>
@@ -401,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,25 +450,286 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>6311.973347009111</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.02194023132324219</v>
+      </c>
+      <c r="I2">
+        <v>0.04687309265136719</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>117.9733470091115</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0.02094268798828125</v>
+      </c>
+      <c r="I3">
+        <v>0.04687309265136719</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2522.026652990888</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0.02090644836425781</v>
+      </c>
+      <c r="I4">
+        <v>0.04883193969726562</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0.1014301971078715</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0.03789901733398438</v>
+      </c>
+      <c r="I5">
+        <v>0.09075546264648438</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>5860.527052656848</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0.02718353271484375</v>
+      </c>
+      <c r="I6">
+        <v>0.0640411376953125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>198.5270526568471</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0.02792167663574219</v>
+      </c>
+      <c r="I7">
+        <v>0.06083488464355469</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2319.472947343153</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0.02393341064453125</v>
+      </c>
+      <c r="I8">
+        <v>0.05684661865234375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
         <v>4</v>
       </c>
-      <c r="F2">
-        <v>18035.4985266037</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0.2393875122070312</v>
-      </c>
-      <c r="I2">
-        <v>0.7479991912841797</v>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>0.1689638276296211</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0.02493476867675781</v>
+      </c>
+      <c r="I9">
+        <v>0.06682205200195312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>5925.849472106609</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0.01296234130859375</v>
+      </c>
+      <c r="I10">
+        <v>0.04986381530761719</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>87.84947210660982</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.01396369934082031</v>
+      </c>
+      <c r="I11">
+        <v>0.06754684448242188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>